<commit_message>
added alberto w/o R; added json aggregation into json; added mamba in config
</commit_message>
<xml_diff>
--- a/data/demo_parameters.xlsx
+++ b/data/demo_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Filenames to Set Mapping"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>set</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>#STD_set_skip</t>
+  </si>
+  <si>
+    <t>sixmix_flag</t>
   </si>
   <si>
     <t>blank</t>
@@ -151,7 +154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,12 +177,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -271,7 +268,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -581,7 +578,7 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -639,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="12"/>
@@ -652,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="12"/>
@@ -665,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="12"/>
@@ -676,7 +673,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -685,7 +682,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -694,7 +691,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -703,7 +700,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -712,7 +709,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -721,7 +718,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -730,7 +727,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -745,7 +742,7 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
app with LCMS-dates in comments
</commit_message>
<xml_diff>
--- a/data/demo_parameters.xlsx
+++ b/data/demo_parameters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>set</t>
   </si>
@@ -95,12 +95,6 @@
     <t>C18H19NO4</t>
   </si>
   <si>
-    <t>Sulfadiamethoxine</t>
-  </si>
-  <si>
-    <t>[M+Na]+</t>
-  </si>
-  <si>
     <t>parameters</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
   </si>
   <si>
     <t>#STD_set_skip</t>
-  </si>
-  <si>
-    <t>sixmix_flag</t>
   </si>
   <si>
     <t>blank</t>
@@ -591,78 +582,78 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="12"/>
@@ -673,7 +664,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -682,7 +673,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -691,7 +682,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -700,7 +691,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -709,7 +700,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -718,7 +709,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -727,7 +718,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -949,19 +940,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
       </c>
       <c r="F8" s="5">
-        <v>198</v>
+        <v>144</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
working workflow;added parameter sheet;added summaries by mz bin; app not compatible
</commit_message>
<xml_diff>
--- a/data/demo_parameters.xlsx
+++ b/data/demo_parameters.xlsx
@@ -4,18 +4,52 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Filenames to Set Mapping"/>
     <sheet r:id="rId2" sheetId="2" name="Standards per Set"/>
+    <sheet r:id="rId3" sheetId="3" name="Other parameters"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Explanations</t>
+  </si>
+  <si>
+    <t>MS1 precision</t>
+  </si>
+  <si>
+    <t>ppm value of MS1 mass precision</t>
+  </si>
+  <si>
+    <t>MS2 precision</t>
+  </si>
+  <si>
+    <t>ppm value of MS2 mass precision</t>
+  </si>
+  <si>
+    <t>Lower mz of mass range</t>
+  </si>
+  <si>
+    <t>here you can put the mz of the lower end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it empty)</t>
+  </si>
+  <si>
+    <t>Upper mz of mass range</t>
+  </si>
+  <si>
+    <t>here you can put the mz of the upper end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it empty)</t>
+  </si>
   <si>
     <t>set</t>
   </si>
@@ -145,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +196,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9c5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -224,42 +264,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -569,156 +612,156 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="133.29071428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="133.29071428571427" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="12"/>
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="10">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="12"/>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4" t="s">
-        <v>34</v>
+      <c r="A7" s="4"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
+      <c r="A8" s="4"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4" t="s">
-        <v>36</v>
+      <c r="A9" s="4"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4" t="s">
-        <v>37</v>
+      <c r="A10" s="4"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4" t="s">
-        <v>38</v>
+      <c r="A11" s="4"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
+      <c r="A12" s="4"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4" t="s">
-        <v>40</v>
+      <c r="A13" s="4"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -737,15 +780,316 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="112.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="112.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>198</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>144</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>138</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>162</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>222</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>276</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="10">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>144</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="10"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="10"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="10"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="11">
+        <f>198/60</f>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="126.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -755,277 +1099,52 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3" s="5">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="4" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>198</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>144</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>138</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>162</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>222</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>276</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="5">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>144</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7">
-        <f>198/60</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added feature MS2 metrics and SQL export
</commit_message>
<xml_diff>
--- a/data/demo_parameters.xlsx
+++ b/data/demo_parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>parameter</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>ppm value of MS2 mass precision</t>
+  </si>
+  <si>
+    <t>Maximum FWHM</t>
+  </si>
+  <si>
+    <t>maximum full width halve maximum value for LC peaks you are interested in in seconds</t>
   </si>
   <si>
     <t>Lower mz of mass range</t>
@@ -201,13 +207,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -264,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -281,31 +287,34 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -616,152 +625,152 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="133.29071428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="133.29071428571427" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="10">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="10">
+        <v>41</v>
+      </c>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="10">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="10">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="10">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4"/>
-      <c r="B13" s="10"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -780,294 +789,294 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="112.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="112.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
-        <v>18</v>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="10">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="11">
+        <v>23</v>
+      </c>
+      <c r="E2" s="12">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="5">
         <v>198</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="9" t="s">
-        <v>22</v>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="10">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="E3" s="12">
         <v>0</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="5">
         <v>144</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>138</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>162</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>222</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>276</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="10">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="12">
         <v>0</v>
       </c>
-      <c r="F4" s="10">
-        <v>138</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="10">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10">
-        <v>162</v>
-      </c>
-      <c r="G5" s="10">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="10">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
-        <v>222</v>
-      </c>
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="10">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10">
-        <v>276</v>
-      </c>
-      <c r="G7" s="10">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="10">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="F8" s="5">
         <v>144</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="5">
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="10"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="10"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="10"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="10"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="10"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="10"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="11">
+      <c r="I14" s="12">
         <f>198/60</f>
       </c>
     </row>
@@ -1081,15 +1090,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="126.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="126.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1125,14 +1134,14 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="6">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1145,6 +1154,17 @@
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handling string arguments in other parameter sheet
</commit_message>
<xml_diff>
--- a/data/demo_parameters.xlsx
+++ b/data/demo_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Filenames to Set Mapping"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>parameter</t>
   </si>
@@ -42,19 +42,25 @@
     <t>Maximum FWHM</t>
   </si>
   <si>
-    <t>maximum full width halve maximum value for LC peaks you are interested in in seconds</t>
+    <t>maximum full width halve maximum value for LC peaks you are interested in in seconds (only used if max and min FWHM above 0)</t>
+  </si>
+  <si>
+    <t>Minimum FWHM</t>
+  </si>
+  <si>
+    <t>minimum full width halve maximum value for LC peaks you are interested in in seconds (only used if max and min FWHM above 0)</t>
   </si>
   <si>
     <t>Lower mz of mass range</t>
   </si>
   <si>
-    <t>here you can put the mz of the lower end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it empty)</t>
+    <t>here you can put the mz of the lower end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it at 0)</t>
   </si>
   <si>
     <t>Upper mz of mass range</t>
   </si>
   <si>
-    <t>here you can put the mz of the upper end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it empty)</t>
+    <t>here you can put the mz of the upper end of your MS1 mass range (for orbitrap this is determined automatically; so you can leave it at 0)</t>
   </si>
   <si>
     <t>set</t>
@@ -216,13 +222,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -296,7 +302,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -308,10 +314,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -325,9 +334,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,38 +639,38 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="28.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="133.29071428571427" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="133.29071428571427" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="7">
+        <v>44</v>
+      </c>
+      <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="4"/>
@@ -672,12 +678,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="7">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5">
         <v>2</v>
       </c>
       <c r="D3" s="4"/>
@@ -685,12 +691,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="4"/>
@@ -698,12 +704,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="7">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5" s="4"/>
@@ -711,12 +717,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="7">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
       </c>
       <c r="D6" s="4"/>
@@ -724,83 +730,83 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="7">
+        <v>51</v>
+      </c>
+      <c r="C10" s="5">
         <v>2</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="14"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -823,290 +829,290 @@
     <col min="2" max="2" style="8" width="22.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="20.719285714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="112.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="112.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="11">
+        <v>25</v>
+      </c>
+      <c r="E2" s="12">
         <v>0</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>198</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="E3" s="12">
         <v>0</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>144</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="11">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
         <v>0</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>138</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="11">
+        <v>25</v>
+      </c>
+      <c r="E5" s="12">
         <v>0</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>162</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="11">
+        <v>25</v>
+      </c>
+      <c r="E6" s="12">
         <v>0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>222</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>1</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="11">
+        <v>25</v>
+      </c>
+      <c r="E7" s="12">
         <v>0</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>276</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>1</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <v>0</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>144</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="7"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="11"/>
+      <c r="I14" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1118,18 +1124,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="126.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="126.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1162,29 +1168,29 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7">
-        <v>20</v>
+      <c r="B4" s="5">
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1193,6 +1199,17 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>